<commit_message>
Je factuur wordt gegenereerd op basis van de bestelling
</commit_message>
<xml_diff>
--- a/webshop/webshop/polls/excelBestanden/facturen/Template2.xlsx
+++ b/webshop/webshop/polls/excelBestanden/facturen/Template2.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -140,10 +142,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,13 +524,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B5:K23"/>
+  <dimension ref="B5:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="5.28515625" customWidth="1" style="1" min="1" max="1"/>
     <col width="4.140625" customWidth="1" style="5" min="2" max="2"/>
@@ -610,15 +612,17 @@
     </row>
     <row r="21">
       <c r="B21" s="8" t="n"/>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>Het werkt</t>
-        </is>
+      <c r="C21" s="7" t="n">
+        <v>6</v>
       </c>
       <c r="E21" s="8" t="n"/>
-      <c r="F21" s="20" t="n"/>
+      <c r="F21" s="20" t="n">
+        <v>44733</v>
+      </c>
       <c r="H21" s="8" t="n"/>
-      <c r="I21" s="21" t="n"/>
+      <c r="I21" s="21" t="n">
+        <v>44738</v>
+      </c>
       <c r="K21" s="8" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -652,8 +656,121 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Snackpan XL</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>35.00</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>35.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Pan</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Aardappel pan</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Subtotaal</t>
+        </is>
+      </c>
+      <c r="J27">
+        <f>J29-J28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>BTW</t>
+        </is>
+      </c>
+      <c r="J28">
+        <f>J29*0.09</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Totaal</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="C23:G23"/>
@@ -664,6 +781,12 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vlg mij was er nog iets gecommit voor de vakantie
</commit_message>
<xml_diff>
--- a/webshop/webshop/polls/excelBestanden/facturen/Template2.xlsx
+++ b/webshop/webshop/polls/excelBestanden/facturen/Template2.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B5:K29"/>
+  <dimension ref="B5:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:E21"/>
@@ -613,15 +613,15 @@
     <row r="21">
       <c r="B21" s="8" t="n"/>
       <c r="C21" s="7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" s="8" t="n"/>
       <c r="F21" s="20" t="n">
-        <v>44733</v>
+        <v>44746</v>
       </c>
       <c r="H21" s="8" t="n"/>
       <c r="I21" s="21" t="n">
-        <v>44738</v>
+        <v>44772</v>
       </c>
       <c r="K21" s="8" t="n"/>
     </row>
@@ -659,17 +659,17 @@
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t>Snackpan XL</t>
+          <t>Pan</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>35.00</t>
+          <t>15.00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -679,98 +679,44 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>35.00</t>
+          <t>45.00</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Pan</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>15.00</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>9%</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>30.00</t>
-        </is>
+          <t>Subtotaal</t>
+        </is>
+      </c>
+      <c r="J25">
+        <f>J27-J26</f>
+        <v/>
       </c>
     </row>
     <row r="26">
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Aardappel pan</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>15.00</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>9%</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>15.00</t>
-        </is>
+          <t>BTW</t>
+        </is>
+      </c>
+      <c r="J26">
+        <f>J27*0.09</f>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="H27" t="inlineStr">
         <is>
-          <t>Subtotaal</t>
-        </is>
-      </c>
-      <c r="J27">
-        <f>J29-J28</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28">
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>BTW</t>
-        </is>
-      </c>
-      <c r="J28">
-        <f>J29*0.09</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29">
-      <c r="H29" t="inlineStr">
-        <is>
           <t>Totaal</t>
         </is>
       </c>
-      <c r="J29" t="n">
-        <v>80</v>
+      <c r="J27" t="n">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="14">
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="C23:G23"/>
@@ -782,11 +728,9 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>